<commit_message>
Updated config, data and excel files.
</commit_message>
<xml_diff>
--- a/application.windows32/data/BIN_volume_cal_meters.xlsx
+++ b/application.windows32/data/BIN_volume_cal_meters.xlsx
@@ -61,9 +61,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +78,21 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -87,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -104,15 +119,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -420,352 +459,355 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>2000</v>
-      </c>
-      <c r="C1">
-        <v>2000</v>
-      </c>
-      <c r="D1">
-        <v>2000</v>
-      </c>
-      <c r="E1">
-        <v>2000</v>
-      </c>
-      <c r="F1">
-        <v>2000</v>
-      </c>
-      <c r="G1">
-        <v>2000</v>
-      </c>
-      <c r="H1">
-        <v>2000</v>
-      </c>
-      <c r="I1">
-        <v>2000</v>
-      </c>
-      <c r="J1">
-        <v>2000</v>
-      </c>
-      <c r="K1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1200</v>
-      </c>
-      <c r="C2">
-        <v>1200</v>
-      </c>
-      <c r="D2">
-        <v>1200</v>
-      </c>
-      <c r="E2">
-        <v>1200</v>
-      </c>
-      <c r="F2">
-        <v>1200</v>
-      </c>
-      <c r="G2">
-        <v>1200</v>
-      </c>
-      <c r="H2">
+      <c r="B2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="H2" s="1">
         <v>1000</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>1000</v>
       </c>
-      <c r="J2">
-        <v>1200</v>
-      </c>
-      <c r="K2">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="J2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>400</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>400</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>400</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>400</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>400</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>400</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>200</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>200</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>400</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>60</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>60</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>60</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>60</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>60</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>60</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>60</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>60</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>60</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>2000</v>
-      </c>
-      <c r="C5">
-        <v>2000</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="1">
         <v>1900</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>1900</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1800</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1800</v>
       </c>
-      <c r="H5">
-        <v>2000</v>
-      </c>
-      <c r="I5">
-        <v>2000</v>
-      </c>
-      <c r="J5">
+      <c r="H5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J5" s="1">
         <v>1850</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
         <v>1850</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>100</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>100</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>100</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>100</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>300</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <f>IF(B$5&gt;B$2,B$3^2*(B$5-B$2),0)+((B$2*B$3/B$2+B$4)^2)/3*B$2-((B$6*B$3/B$2+B$4)^2)/3*B$6</f>
         <v>212640000</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <f t="shared" ref="C7:K7" si="0">IF(C$5&gt;C$2,C$3^2*(C$5-C$2),0)+((C$2*C$3/C$2+C$4)^2)/3*C$2-((C$6*C$3/C$2+C$4)^2)/3*C$6</f>
         <v>212349629.62962964</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
         <v>196640000</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>196349629.62962964</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>180640000</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>180349629.62962964</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
         <v>62533333.333333328</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>62319999.999999993</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="4">
         <f t="shared" si="0"/>
         <v>186080000</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
         <v>183656296.2962963</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>1200</v>
-      </c>
-      <c r="C8">
-        <v>1200</v>
-      </c>
-      <c r="D8">
-        <v>1200</v>
-      </c>
-      <c r="E8">
-        <v>1200</v>
-      </c>
-      <c r="F8">
-        <v>1200</v>
-      </c>
-      <c r="G8">
-        <v>1200</v>
-      </c>
-      <c r="H8">
-        <v>1200</v>
-      </c>
-      <c r="I8">
-        <v>1200</v>
-      </c>
-      <c r="J8">
-        <v>1200</v>
-      </c>
-      <c r="K8">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <f t="shared" ref="B9:K9" si="1">IF(B8&gt;B$2,IF(B8&gt;B$5,B$3^2*(B$5-B$2),B$3^2*(B8-B$2)),0)+IF(B8&gt;=B$2,((B$2*B$3/B$2+B$4)^2)/3*B$2-((B$6*B$3/B$2+B$4)^2)/3*B$6,IF(B8&gt;B$6,((B8*B$3/B$2+B$4)^2)/3*B8-((B$6*B$3/B$2+B$4)^2)/3*B$6,0))</f>
         <v>84640000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <f t="shared" si="1"/>
         <v>84349629.629629627</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <f t="shared" si="1"/>
         <v>84640000</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <f t="shared" si="1"/>
         <v>84349629.629629627</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>84640000</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>84349629.629629627</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>30533333.333333332</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <f t="shared" si="1"/>
         <v>30320000</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="5">
         <f t="shared" si="1"/>
         <v>82080000</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="5">
         <f t="shared" si="1"/>
         <v>79656296.296296299</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3">
@@ -809,88 +851,88 @@
         <v>0.4337248322147651</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>500</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>500</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>500</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>500</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>500</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>500</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>500</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>500</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>500</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <f t="shared" ref="B12:K12" si="3">IF(B11&gt;B$2,IF(B11&gt;B$5,B$3^2*(B$5-B$2),B$3^2*(B11-B$2)),0)+IF(B11&gt;=B$2,((B$2*B$3/B$2+B$4)^2)/3*B$2-((B$6*B$3/B$2+B$4)^2)/3*B$6,IF(B11&gt;B$6,((B11*B$3/B$2+B$4)^2)/3*B11-((B$6*B$3/B$2+B$4)^2)/3*B$6,0))</f>
         <v>8562962.9629629608</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <f t="shared" si="3"/>
         <v>8272592.5925925905</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <f t="shared" si="3"/>
         <v>8562962.9629629608</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <f t="shared" si="3"/>
         <v>8272592.5925925905</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <f t="shared" si="3"/>
         <v>8562962.9629629608</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <f t="shared" si="3"/>
         <v>8272592.5925925905</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <f t="shared" si="3"/>
         <v>4266666.666666667</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <f t="shared" si="3"/>
         <v>4053333.3333333335</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="5">
         <f t="shared" si="3"/>
         <v>6002962.9629629608</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <f t="shared" si="3"/>
         <v>3579259.2592592565</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3">
@@ -934,88 +976,88 @@
         <v>1.9488900361383569E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1900</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>1900</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>1900</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>1900</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>1900</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>1900</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>1900</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>1900</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>1900</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="1">
         <v>1900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <f t="shared" ref="B15:K15" si="5">IF(B14&gt;B$2,IF(B14&gt;B$5,B$3^2*(B$5-B$2),B$3^2*(B14-B$2)),0)+IF(B14&gt;=B$2,((B$2*B$3/B$2+B$4)^2)/3*B$2-((B$6*B$3/B$2+B$4)^2)/3*B$6,IF(B14&gt;B$6,((B14*B$3/B$2+B$4)^2)/3*B14-((B$6*B$3/B$2+B$4)^2)/3*B$6,0))</f>
         <v>196640000</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <f t="shared" si="5"/>
         <v>196349629.62962961</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <f t="shared" si="5"/>
         <v>196640000</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <f t="shared" si="5"/>
         <v>196349629.62962961</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="5">
         <f t="shared" si="5"/>
         <v>180640000</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="5">
         <f t="shared" si="5"/>
         <v>180349629.62962961</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <f t="shared" si="5"/>
         <v>58533333.333333328</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <f t="shared" si="5"/>
         <v>58320000</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="5">
         <f t="shared" si="5"/>
         <v>186080000</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="5">
         <f t="shared" si="5"/>
         <v>183656296.2962963</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="3">
@@ -1059,88 +1101,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>200</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>200</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>200</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>200</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>200</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>200</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>200</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>200</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>200</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <f t="shared" ref="B18:I18" si="7">IF(B17&gt;B$2,IF(B17&gt;B$5,B$3^2*(B$5-B$2),B$3^2*(B17-B$2)),0)+IF(B17&gt;=B$2,((B$2*B$3/B$2+B$4)^2)/3*B$2-((B$6*B$3/B$2+B$4)^2)/3*B$6,IF(B17&gt;B$6,((B17*B$3/B$2+B$4)^2)/3*B17-((B$6*B$3/B$2+B$4)^2)/3*B$6,0))</f>
         <v>1069629.6296296297</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <f t="shared" si="7"/>
         <v>779259.25925925921</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <f t="shared" si="7"/>
         <v>1069629.6296296297</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <f t="shared" si="7"/>
         <v>779259.25925925921</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="5">
         <f t="shared" si="7"/>
         <v>1069629.6296296297</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="5">
         <f t="shared" si="7"/>
         <v>779259.25925925921</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <f t="shared" si="7"/>
         <v>666666.66666666674</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <f t="shared" si="7"/>
         <v>453333.33333333337</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="5">
         <f>IF(J17&gt;J$2,IF(J17&gt;J$5,J$3^2*(J$5-J$2),J$3^2*(J17-J$2)),0)+IF(J17&gt;=J$2,((J$2*J$3/J$2+J$4)^2)/3*J$2-((J$6*J$3/J$2+J$4)^2)/3*J$6,IF(J17&gt;J$6,((J17*J$3/J$2+J$4)^2)/3*J17-((J$6*J$3/J$2+J$4)^2)/3*J$6,0))</f>
         <v>0</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="5">
         <f t="shared" ref="K18" si="8">IF(K17&gt;K$2,IF(K17&gt;K$5,K$3^2*(K$5-K$2),K$3^2*(K17-K$2)),0)+IF(K17&gt;=K$2,((K$2*K$3/K$2+K$4)^2)/3*K$2-((K$6*K$3/K$2+K$4)^2)/3*K$6,IF(K17&gt;K$6,((K17*K$3/K$2+K$4)^2)/3*K17-((K$6*K$3/K$2+K$4)^2)/3*K$6,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="3">

</xml_diff>